<commit_message>
Add coal supply curve
</commit_message>
<xml_diff>
--- a/nature14016-f1.xlsx
+++ b/nature14016-f1.xlsx
@@ -9,13 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="7260" yWindow="460" windowWidth="23520" windowHeight="13760" activeTab="1"/>
+    <workbookView xWindow="700" yWindow="460" windowWidth="24900" windowHeight="13760" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Fig 1" sheetId="1" r:id="rId1"/>
-    <sheet name="Oil data" sheetId="2" r:id="rId2"/>
+    <sheet name="Coal data" sheetId="4" r:id="rId2"/>
+    <sheet name="Oil data" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="150001" calcMode="manual" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="996" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1073" uniqueCount="40">
   <si>
     <t>Panel a</t>
   </si>
@@ -668,8 +669,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X487"/>
   <sheetViews>
-    <sheetView topLeftCell="A332" zoomScaleNormal="55" zoomScalePageLayoutView="55" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:D332"/>
+    <sheetView topLeftCell="H1" zoomScaleNormal="55" zoomScalePageLayoutView="55" workbookViewId="0">
+      <selection activeCell="L1" sqref="L1:N1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7781,9 +7782,854 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C75"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="57.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.1640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.1640625" style="5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="23" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="5">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="C2" s="24">
+        <v>0.82899999999999996</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="5">
+        <v>0.27500000000000002</v>
+      </c>
+      <c r="C3" s="5">
+        <v>0.93400000000000005</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="5">
+        <v>2.1000000000000001E-2</v>
+      </c>
+      <c r="C4" s="5">
+        <v>1.145</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="5">
+        <v>0.114</v>
+      </c>
+      <c r="C5" s="5">
+        <v>1.2549999999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="5">
+        <v>0</v>
+      </c>
+      <c r="C6" s="5">
+        <v>1.3560000000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="5">
+        <v>9.6000000000000002E-2</v>
+      </c>
+      <c r="C7" s="5">
+        <v>1.4790000000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="5">
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="C8" s="5">
+        <v>1.4810000000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="5">
+        <v>1.085</v>
+      </c>
+      <c r="C9" s="5">
+        <v>1.524</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="5">
+        <v>0.40300000000000002</v>
+      </c>
+      <c r="C10" s="5">
+        <v>1.546</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="5">
+        <v>0.438</v>
+      </c>
+      <c r="C11" s="5">
+        <v>1.629</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" s="5">
+        <v>0.221</v>
+      </c>
+      <c r="C12" s="5">
+        <v>1.6870000000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" s="5">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="C13" s="5">
+        <v>1.86</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" s="5">
+        <v>0.11700000000000001</v>
+      </c>
+      <c r="C14" s="5">
+        <v>1.929</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" s="5">
+        <v>0.39500000000000002</v>
+      </c>
+      <c r="C15" s="5">
+        <v>1.9610000000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" s="5">
+        <v>2.7E-2</v>
+      </c>
+      <c r="C16" s="5">
+        <v>2.1030000000000002</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B17" s="5">
+        <v>1.2050000000000001</v>
+      </c>
+      <c r="C17" s="5">
+        <v>2.274</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B18" s="5">
+        <v>0.76700000000000002</v>
+      </c>
+      <c r="C18" s="5">
+        <v>2.335</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19" s="5">
+        <v>5.8330000000000002</v>
+      </c>
+      <c r="C19" s="5">
+        <v>2.407</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B20" s="5">
+        <v>2.4E-2</v>
+      </c>
+      <c r="C20" s="5">
+        <v>2.4940000000000002</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B21" s="5">
+        <v>3.016</v>
+      </c>
+      <c r="C21" s="5">
+        <v>2.7650000000000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B22" s="5">
+        <v>0.104</v>
+      </c>
+      <c r="C22" s="5">
+        <v>3.0310000000000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B23" s="5">
+        <v>5.5990000000000002</v>
+      </c>
+      <c r="C23" s="5">
+        <v>3.06</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B24" s="5">
+        <v>0.23699999999999999</v>
+      </c>
+      <c r="C24" s="5">
+        <v>3.2730000000000001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B25" s="5">
+        <v>0.185</v>
+      </c>
+      <c r="C25" s="5">
+        <v>3.306</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B26" s="5">
+        <v>0.37</v>
+      </c>
+      <c r="C26" s="5">
+        <v>3.3540000000000001</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B27" s="5">
+        <v>1.2E-2</v>
+      </c>
+      <c r="C27" s="5">
+        <v>3.4470000000000001</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B28" s="5">
+        <v>0.57199999999999995</v>
+      </c>
+      <c r="C28" s="5">
+        <v>3.6179999999999999</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B29" s="5">
+        <v>0.106</v>
+      </c>
+      <c r="C29" s="5">
+        <v>3.6789999999999998</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B30" s="5">
+        <v>5.9219999999999997</v>
+      </c>
+      <c r="C30" s="5">
+        <v>3.7519999999999998</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B31" s="5">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="C31" s="5">
+        <v>3.839</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B32" s="5">
+        <v>1.6E-2</v>
+      </c>
+      <c r="C32" s="5">
+        <v>3.8879999999999999</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B33" s="5">
+        <v>3.5720000000000001</v>
+      </c>
+      <c r="C33" s="5">
+        <v>4.109</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B34" s="24">
+        <v>0.108</v>
+      </c>
+      <c r="C34" s="24">
+        <v>4.1900000000000004</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B35" s="5">
+        <v>0.80900000000000005</v>
+      </c>
+      <c r="C35" s="5">
+        <v>4.2949999999999999</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B36" s="5">
+        <v>2.5779999999999998</v>
+      </c>
+      <c r="C36" s="5">
+        <v>4.4039999999999999</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B37" s="5">
+        <v>0</v>
+      </c>
+      <c r="C37" s="5">
+        <v>4.4249999999999998</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B38" s="5">
+        <v>5.7000000000000002E-2</v>
+      </c>
+      <c r="C38" s="5">
+        <v>4.4809999999999999</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B39" s="5">
+        <v>2E-3</v>
+      </c>
+      <c r="C39" s="5">
+        <v>4.5060000000000002</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B40" s="5">
+        <v>1E-3</v>
+      </c>
+      <c r="C40" s="5">
+        <v>4.5149999999999997</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B41" s="5">
+        <v>0.437</v>
+      </c>
+      <c r="C41" s="5">
+        <v>4.6159999999999997</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B42" s="5">
+        <v>0.23799999999999999</v>
+      </c>
+      <c r="C42" s="5">
+        <v>4.6989999999999998</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B43" s="5">
+        <v>0.249</v>
+      </c>
+      <c r="C43" s="5">
+        <v>4.84</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A44" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B44" s="5">
+        <v>1.2E-2</v>
+      </c>
+      <c r="C44" s="5">
+        <v>4.8419999999999996</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A45" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B45" s="5">
+        <v>1.3540000000000001</v>
+      </c>
+      <c r="C45" s="5">
+        <v>4.8849999999999998</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A46" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B46" s="5">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="C46" s="5">
+        <v>4.907</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A47" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B47" s="5">
+        <v>0.46100000000000002</v>
+      </c>
+      <c r="C47" s="5">
+        <v>4.99</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A48" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B48" s="5">
+        <v>2.4E-2</v>
+      </c>
+      <c r="C48" s="5">
+        <v>5.2210000000000001</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A49" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B49" s="5">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="C49" s="5">
+        <v>5.8259999999999996</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A50" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B50" s="5">
+        <v>0.24299999999999999</v>
+      </c>
+      <c r="C50" s="5">
+        <v>6.0629999999999997</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A51" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B51" s="5">
+        <v>0.55200000000000005</v>
+      </c>
+      <c r="C51" s="5">
+        <v>6.5460000000000003</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A52" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B52" s="5">
+        <v>0.43099999999999999</v>
+      </c>
+      <c r="C52" s="5">
+        <v>6.6109999999999998</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A53" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B53" s="5">
+        <v>2.8000000000000001E-2</v>
+      </c>
+      <c r="C53" s="5">
+        <v>6.8949999999999996</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A54" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B54" s="5">
+        <v>1.3340000000000001</v>
+      </c>
+      <c r="C54" s="5">
+        <v>7.2359999999999998</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A55" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B55" s="5">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="C55" s="5">
+        <v>7.2489999999999997</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A56" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B56" s="5">
+        <v>0.248</v>
+      </c>
+      <c r="C56" s="5">
+        <v>7.3579999999999997</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A57" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B57" s="5">
+        <v>13.818</v>
+      </c>
+      <c r="C57" s="5">
+        <v>7.5039999999999996</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A58" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B58" s="5">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="C58" s="5">
+        <v>7.6769999999999996</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A59" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B59" s="5">
+        <v>8.3350000000000009</v>
+      </c>
+      <c r="C59" s="5">
+        <v>8.218</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A60" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B60" s="24">
+        <v>0.251</v>
+      </c>
+      <c r="C60" s="24">
+        <v>8.3800000000000008</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A61" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B61" s="5">
+        <v>1.887</v>
+      </c>
+      <c r="C61" s="5">
+        <v>8.5909999999999993</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A62" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B62" s="5">
+        <v>6.0149999999999997</v>
+      </c>
+      <c r="C62" s="5">
+        <v>8.8079999999999998</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A63" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B63" s="5">
+        <v>1E-3</v>
+      </c>
+      <c r="C63" s="5">
+        <v>8.8510000000000009</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A64" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B64" s="5">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="C64" s="5">
+        <v>9.0120000000000005</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A65" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B65" s="5">
+        <v>2E-3</v>
+      </c>
+      <c r="C65" s="5">
+        <v>9.0299999999999994</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A66" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B66" s="5">
+        <v>1.0189999999999999</v>
+      </c>
+      <c r="C66" s="5">
+        <v>9.2319999999999993</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A67" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B67" s="5">
+        <v>0.55500000000000005</v>
+      </c>
+      <c r="C67" s="5">
+        <v>9.3970000000000002</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A68" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B68" s="5">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="C68" s="5">
+        <v>9.68</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A69" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B69" s="5">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="C69" s="5">
+        <v>9.6839999999999993</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A70" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B70" s="5">
+        <v>3.1579999999999999</v>
+      </c>
+      <c r="C70" s="5">
+        <v>9.7690000000000001</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A71" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B71" s="5">
+        <v>8.1000000000000003E-2</v>
+      </c>
+      <c r="C71" s="5">
+        <v>9.8140000000000001</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A72" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B72" s="5">
+        <v>1.075</v>
+      </c>
+      <c r="C72" s="5">
+        <v>9.98</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A73" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B73" s="5">
+        <v>5.7000000000000002E-2</v>
+      </c>
+      <c r="C73" s="5">
+        <v>10.442</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A74" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B74" s="5">
+        <v>0.16200000000000001</v>
+      </c>
+      <c r="C74" s="5">
+        <v>11.651</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A75" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B75" s="5">
+        <v>0.02</v>
+      </c>
+      <c r="C75" s="5">
+        <v>14.497</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C328"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>

</xml_diff>